<commit_message>
Update unit test for hasFile fix
Signed-off-by: Gary O'Neall <gary@sourceauditor.com>
</commit_message>
<xml_diff>
--- a/testResources/SPDXSpreadsheetExample-v2.2.xlsx
+++ b/testResources/SPDXSpreadsheetExample-v2.2.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gary\git\tools-java\testResources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF92040A-8108-4A8C-8CAE-FA4464F7315F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Document Info" r:id="rId3" sheetId="1"/>
-    <sheet name="Package Info" r:id="rId4" sheetId="2"/>
-    <sheet name="External Refs" r:id="rId5" sheetId="3"/>
-    <sheet name="Extracted License Info" r:id="rId6" sheetId="4"/>
-    <sheet name="Per File Info" r:id="rId7" sheetId="5"/>
-    <sheet name="Relationships" r:id="rId8" sheetId="6"/>
-    <sheet name="Annotations" r:id="rId9" sheetId="7"/>
-    <sheet name="Snippets" r:id="rId10" sheetId="8"/>
-    <sheet name="Reviewers" r:id="rId11" sheetId="9"/>
+    <sheet name="Document Info" sheetId="1" r:id="rId1"/>
+    <sheet name="Package Info" sheetId="2" r:id="rId2"/>
+    <sheet name="External Refs" sheetId="3" r:id="rId3"/>
+    <sheet name="Extracted License Info" sheetId="4" r:id="rId4"/>
+    <sheet name="Per File Info" sheetId="5" r:id="rId5"/>
+    <sheet name="Relationships" sheetId="6" r:id="rId6"/>
+    <sheet name="Annotations" sheetId="7" r:id="rId7"/>
+    <sheet name="Snippets" sheetId="8" r:id="rId8"/>
+    <sheet name="Reviewers" sheetId="9" r:id="rId9"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="211">
   <si>
     <t>Spreadsheet Version</t>
   </si>
@@ -767,147 +775,75 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="19">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
       <name val="Arial"/>
-      <sz val="10.0"/>
-      <b val="true"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
-    </font>
-    <font>
-      <name val="Wingdings 2"/>
-      <sz val="10.0"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="darkGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="22"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="43"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="43"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -915,254 +851,427 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="false" horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.0" customWidth="true" style="2"/>
-    <col min="2" max="2" width="16.0" customWidth="true" style="2"/>
-    <col min="3" max="3" width="20.0" customWidth="true" style="2"/>
-    <col min="4" max="4" width="20.0" customWidth="true" style="2"/>
-    <col min="5" max="5" width="16.0" customWidth="true" style="2"/>
-    <col min="6" max="6" width="40.0" customWidth="true" style="3"/>
-    <col min="7" max="7" width="80.0" customWidth="true" style="3"/>
-    <col min="8" max="8" width="50.0" customWidth="true" style="3"/>
-    <col min="9" max="9" width="140.0" customWidth="true" style="3"/>
-    <col min="10" max="10" width="70.0" customWidth="true" style="3"/>
-    <col min="11" max="11" width="60.0" customWidth="true" style="3"/>
-    <col min="12" max="12" width="20.0" customWidth="true" style="2"/>
-    <col min="13" max="13" width="70.0" customWidth="true" style="3"/>
-    <col min="14" max="14" width="60.0" customWidth="true" style="3"/>
+    <col min="1" max="1" width="20" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40" style="3" customWidth="1"/>
+    <col min="7" max="7" width="80" style="3" customWidth="1"/>
+    <col min="8" max="8" width="50" style="3" customWidth="1"/>
+    <col min="9" max="9" width="140" style="3" customWidth="1"/>
+    <col min="10" max="10" width="70" style="3" customWidth="1"/>
+    <col min="11" max="11" width="60" style="3" customWidth="1"/>
+    <col min="12" max="12" width="20" style="2" customWidth="1"/>
+    <col min="13" max="13" width="70" style="3" customWidth="1"/>
+    <col min="14" max="14" width="60" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" ht="24.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1240,14 +1349,14 @@
       <c r="K2" t="s">
         <v>81</v>
       </c>
-      <c r="L2" t="n" s="28">
-        <v>40207.77108796296</v>
+      <c r="L2" s="27">
+        <v>40207.771087962959</v>
       </c>
       <c r="M2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="H3" t="s">
         <v>91</v>
       </c>
@@ -1255,50 +1364,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="K4" t="s">
         <v>83</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.0" customWidth="true" style="5"/>
-    <col min="2" max="2" width="17.0" customWidth="true" style="5"/>
-    <col min="3" max="3" width="17.0" customWidth="true" style="5"/>
-    <col min="4" max="4" width="30.0" customWidth="true" style="5"/>
-    <col min="5" max="5" width="30.0" customWidth="true" style="5"/>
-    <col min="6" max="6" width="30.0" customWidth="true" style="5"/>
-    <col min="7" max="7" width="50.0" customWidth="true" style="5"/>
-    <col min="8" max="8" width="50.0" customWidth="true" style="5"/>
-    <col min="9" max="9" width="75.0" customWidth="true" style="5"/>
-    <col min="10" max="10" width="60.0" customWidth="true" style="5"/>
-    <col min="11" max="11" width="40.0" customWidth="true" style="5"/>
-    <col min="12" max="12" width="30.0" customWidth="true" style="5"/>
-    <col min="13" max="13" width="40.0" customWidth="true" style="5"/>
-    <col min="14" max="14" width="40.0" customWidth="true" style="5"/>
-    <col min="15" max="15" width="90.0" customWidth="true" style="5"/>
-    <col min="16" max="16" width="50.0" customWidth="true" style="5"/>
-    <col min="17" max="17" width="50.0" customWidth="true" style="5"/>
-    <col min="18" max="18" width="50.0" customWidth="true" style="5"/>
-    <col min="19" max="19" width="80.0" customWidth="true" style="5"/>
-    <col min="20" max="20" width="80.0" customWidth="true" style="5"/>
-    <col min="21" max="21" width="10.0" customWidth="true" style="5"/>
-    <col min="22" max="22" width="50.0" customWidth="true" style="5"/>
-    <col min="23" max="23" width="50.0" customWidth="true" style="5"/>
+    <col min="1" max="1" width="30" style="5" customWidth="1"/>
+    <col min="2" max="3" width="17" style="5" customWidth="1"/>
+    <col min="4" max="6" width="30" style="5" customWidth="1"/>
+    <col min="7" max="8" width="50" style="5" customWidth="1"/>
+    <col min="9" max="9" width="75" style="5" customWidth="1"/>
+    <col min="10" max="10" width="60" style="5" customWidth="1"/>
+    <col min="11" max="11" width="40" style="5" customWidth="1"/>
+    <col min="12" max="12" width="30" style="5" customWidth="1"/>
+    <col min="13" max="14" width="40" style="5" customWidth="1"/>
+    <col min="15" max="15" width="90" style="5" customWidth="1"/>
+    <col min="16" max="18" width="50" style="5" customWidth="1"/>
+    <col min="19" max="20" width="80" style="5" customWidth="1"/>
+    <col min="21" max="21" width="10" style="5" customWidth="1"/>
+    <col min="22" max="23" width="50" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30.0" customHeight="true">
+    <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1369,7 +1469,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -1406,7 +1506,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>100</v>
       </c>
@@ -1471,7 +1571,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -1508,7 +1608,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1554,27 +1654,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.0" customWidth="true" style="7"/>
-    <col min="2" max="2" width="25.0" customWidth="true" style="7"/>
-    <col min="3" max="3" width="40.0" customWidth="true" style="8"/>
-    <col min="4" max="4" width="60.0" customWidth="true" style="8"/>
-    <col min="5" max="5" width="40.0" customWidth="true" style="8"/>
-    <col min="6" max="6" width="40.0" customWidth="true" style="8"/>
+    <col min="1" max="2" width="25" style="7" customWidth="1"/>
+    <col min="3" max="3" width="40" style="8" customWidth="1"/>
+    <col min="4" max="4" width="60" style="8" customWidth="1"/>
+    <col min="5" max="6" width="40" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>38</v>
       </c>
@@ -1594,7 +1692,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -1608,7 +1706,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1626,27 +1724,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.0" customWidth="true" style="10"/>
-    <col min="2" max="2" width="120.0" customWidth="true"/>
-    <col min="3" max="3" width="50.0" customWidth="true" style="10"/>
-    <col min="4" max="4" width="80.0" customWidth="true" style="11"/>
-    <col min="5" max="5" width="80.0" customWidth="true" style="11"/>
-    <col min="6" max="6" width="50.0" customWidth="true" style="11"/>
+    <col min="1" max="1" width="15" style="10" customWidth="1"/>
+    <col min="2" max="2" width="120" customWidth="1"/>
+    <col min="3" max="3" width="50" style="10" customWidth="1"/>
+    <col min="4" max="5" width="80" style="11" customWidth="1"/>
+    <col min="6" max="6" width="50" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="9" t="s">
         <v>44</v>
       </c>
@@ -1666,7 +1763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1674,7 +1771,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -1682,7 +1779,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -1690,7 +1787,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -1698,7 +1795,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -1716,39 +1813,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="60.0" customWidth="true" style="14"/>
-    <col min="2" max="2" width="25.0" customWidth="true" style="13"/>
-    <col min="3" max="3" width="25.0" customWidth="true" style="13"/>
-    <col min="4" max="4" width="30.0" customWidth="true" style="14"/>
-    <col min="5" max="5" width="85.0" customWidth="true" style="14"/>
-    <col min="6" max="6" width="50.0" customWidth="true" style="14"/>
-    <col min="7" max="7" width="50.0" customWidth="true" style="14"/>
-    <col min="8" max="8" width="60.0" customWidth="true" style="14"/>
-    <col min="9" max="9" width="70.0" customWidth="true" style="14"/>
-    <col min="10" max="10" width="70.0" customWidth="true" style="14"/>
-    <col min="11" max="11" width="35.0" customWidth="true" style="14"/>
-    <col min="12" max="12" width="60.0" customWidth="true" style="14"/>
-    <col min="13" max="13" width="60.0" customWidth="true" style="14"/>
-    <col min="14" max="14" width="60.0" customWidth="true" style="14"/>
-    <col min="15" max="15" width="60.0" customWidth="true" style="14"/>
-    <col min="16" max="16" width="60.0" customWidth="true" style="14"/>
-    <col min="17" max="17" width="60.0" customWidth="true" style="14"/>
-    <col min="18" max="18" width="60.0" customWidth="true" style="14"/>
+    <col min="1" max="1" width="60" style="14" customWidth="1"/>
+    <col min="2" max="3" width="25" style="13" customWidth="1"/>
+    <col min="4" max="4" width="30" style="14" customWidth="1"/>
+    <col min="5" max="5" width="85" style="14" customWidth="1"/>
+    <col min="6" max="7" width="50" style="14" customWidth="1"/>
+    <col min="8" max="8" width="60" style="14" customWidth="1"/>
+    <col min="9" max="10" width="70" style="14" customWidth="1"/>
+    <col min="11" max="11" width="35" style="14" customWidth="1"/>
+    <col min="12" max="18" width="60" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="12" t="s">
         <v>48</v>
       </c>
@@ -1804,7 +1892,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>156</v>
       </c>
@@ -1839,7 +1927,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>164</v>
       </c>
@@ -1874,7 +1962,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -1909,7 +1997,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>180</v>
       </c>
@@ -1939,26 +2027,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="20.0" customWidth="true" style="16"/>
-    <col min="2" max="2" width="25.0" customWidth="true" style="16"/>
-    <col min="3" max="3" width="20.0" customWidth="true" style="16"/>
-    <col min="4" max="4" width="70.0" customWidth="true" style="17"/>
-    <col min="5" max="5" width="50.0" customWidth="true" style="17"/>
+    <col min="1" max="1" width="20" style="16" customWidth="1"/>
+    <col min="2" max="2" width="25" style="16" customWidth="1"/>
+    <col min="3" max="3" width="20" style="16" customWidth="1"/>
+    <col min="4" max="4" width="70" style="17" customWidth="1"/>
+    <col min="5" max="5" width="50" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="15" t="s">
         <v>61</v>
       </c>
@@ -1975,7 +2065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>154</v>
       </c>
@@ -1986,7 +2076,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1997,7 +2087,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -2008,7 +2098,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -2019,7 +2109,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -2030,7 +2120,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -2041,7 +2131,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>163</v>
       </c>
@@ -2052,50 +2142,39 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" t="s">
-        <v>196</v>
-      </c>
-      <c r="C10" t="s">
         <v>124</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.0" customWidth="true" style="19"/>
-    <col min="2" max="2" width="70.0" customWidth="true" style="20"/>
-    <col min="3" max="3" width="25.0" customWidth="true" style="19"/>
-    <col min="4" max="4" width="60.0" customWidth="true" style="20"/>
-    <col min="5" max="5" width="20.0" customWidth="true" style="19"/>
-    <col min="6" max="6" width="50.0" customWidth="true" style="20"/>
+    <col min="1" max="1" width="25" style="19" customWidth="1"/>
+    <col min="2" max="2" width="70" style="20" customWidth="1"/>
+    <col min="3" max="3" width="25" style="19" customWidth="1"/>
+    <col min="4" max="4" width="60" style="20" customWidth="1"/>
+    <col min="5" max="5" width="20" style="19" customWidth="1"/>
+    <col min="6" max="6" width="50" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30.0" customHeight="true">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="18" t="s">
         <v>65</v>
       </c>
@@ -2115,7 +2194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -2132,7 +2211,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -2149,7 +2228,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -2166,7 +2245,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>90</v>
       </c>
@@ -2183,7 +2262,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>91</v>
       </c>
@@ -2201,32 +2280,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.0" customWidth="true" style="22"/>
-    <col min="2" max="2" width="25.0" customWidth="true" style="22"/>
-    <col min="3" max="3" width="25.0" customWidth="true" style="22"/>
-    <col min="4" max="4" width="40.0" customWidth="true" style="22"/>
-    <col min="5" max="5" width="40.0" customWidth="true" style="22"/>
-    <col min="6" max="6" width="60.0" customWidth="true" style="23"/>
-    <col min="7" max="7" width="60.0" customWidth="true" style="23"/>
-    <col min="8" max="8" width="60.0" customWidth="true" style="23"/>
-    <col min="9" max="9" width="60.0" customWidth="true" style="23"/>
-    <col min="10" max="10" width="60.0" customWidth="true" style="23"/>
-    <col min="11" max="11" width="40.0" customWidth="true" style="23"/>
+    <col min="1" max="3" width="25" style="22" customWidth="1"/>
+    <col min="4" max="5" width="40" style="22" customWidth="1"/>
+    <col min="6" max="10" width="60" style="23" customWidth="1"/>
+    <col min="11" max="11" width="40" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="21" t="s">
         <v>70</v>
       </c>
@@ -2261,7 +2333,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>184</v>
       </c>
@@ -2294,24 +2366,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="60.0" customWidth="true" style="26"/>
-    <col min="2" max="2" width="20.0" customWidth="true" style="25"/>
-    <col min="3" max="3" width="120.0" customWidth="true" style="26"/>
+    <col min="1" max="1" width="60" style="26" customWidth="1"/>
+    <col min="2" max="2" width="20" style="25" customWidth="1"/>
+    <col min="3" max="3" width="120" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="24" t="s">
         <v>77</v>
       </c>
@@ -2323,6 +2395,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>